<commit_message>
Refactor laporan views to update damage categories and impacts, enhance UI with new styles, and improve user feedback. Remove unused routes for kategori_kerusakan and add new routes for duplicate checks and voting functionality.
</commit_message>
<xml_diff>
--- a/public/assets/excel/template_data_fasilitas.xlsx
+++ b/public/assets/excel/template_data_fasilitas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PBL-SEMESTER04\PBL-Fasilita\public\assets\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PBL-Fasilita\public\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A2A4E22-A3F1-4A95-ABD9-650DDF8E96A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A6074E-D830-4B0F-B457-0CACCEAA9262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{33A30061-6107-4F2C-A2C0-30C64088051A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{33A30061-6107-4F2C-A2C0-30C64088051A}"/>
   </bookViews>
   <sheets>
     <sheet name="Lembar1" sheetId="1" r:id="rId1"/>
@@ -34,12 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">nama fasilitas </t>
-  </si>
-  <si>
-    <t>jumlah</t>
   </si>
   <si>
     <t>id_kategori</t>
@@ -129,7 +126,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -428,7 +425,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -439,25 +436,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3">
         <v>2</v>
       </c>
+      <c r="C2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>